<commit_message>
Add local update to file
</commit_message>
<xml_diff>
--- a/RPADev-S04P02-CalculatingLossInvoices-Invoices.xlsx
+++ b/RPADev-S04P02-CalculatingLossInvoices-Invoices.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE64C4A-A37A-4D96-A549-C928277C859B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14340" windowHeight="12525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,7 +93,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -405,20 +404,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,7 +426,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -440,7 +437,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -451,7 +448,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -462,7 +459,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -473,7 +470,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -484,7 +481,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -495,7 +492,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -506,7 +503,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -517,7 +514,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -528,7 +525,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -539,7 +536,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -550,7 +547,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -561,7 +558,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -572,7 +569,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -583,7 +580,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -594,7 +591,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -605,7 +602,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -616,7 +613,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -627,7 +624,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -638,7 +635,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -649,7 +646,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -660,7 +657,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -671,7 +668,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -682,7 +679,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -693,7 +690,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -704,7 +701,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -715,7 +712,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -726,7 +723,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -737,7 +734,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -748,7 +745,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -759,7 +756,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -770,7 +767,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -781,7 +778,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -792,7 +789,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -803,7 +800,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -814,7 +811,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -825,7 +822,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -836,7 +833,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -847,7 +844,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -858,7 +855,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -869,7 +866,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -880,7 +877,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -891,7 +888,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -902,7 +899,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -913,7 +910,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -924,7 +921,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -935,7 +932,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -946,7 +943,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -957,7 +954,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -968,7 +965,7 @@
         <v>4120</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -979,7 +976,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -990,7 +987,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1001,7 +998,7 @@
         <v>6320</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1012,7 +1009,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1023,7 +1020,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1034,7 +1031,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1045,7 +1042,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1056,7 +1053,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1067,7 +1064,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1078,7 +1075,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1089,7 +1086,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1100,7 +1097,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1111,7 +1108,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1122,7 +1119,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1133,7 +1130,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1144,7 +1141,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1155,7 +1152,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1166,7 +1163,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1177,7 +1174,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1188,7 +1185,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1199,7 +1196,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1210,7 +1207,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1221,7 +1218,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1232,7 +1229,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1243,7 +1240,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1254,7 +1251,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -1265,7 +1262,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -1276,7 +1273,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -1287,7 +1284,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -1298,7 +1295,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -1309,7 +1306,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -1320,7 +1317,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -1331,7 +1328,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -1342,7 +1339,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -1353,7 +1350,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -1364,7 +1361,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -1375,7 +1372,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -1386,7 +1383,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -1397,7 +1394,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -1408,7 +1405,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -1419,7 +1416,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -1430,7 +1427,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -1441,7 +1438,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -1452,7 +1449,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -1463,7 +1460,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -1474,7 +1471,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -1485,7 +1482,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -1496,7 +1493,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -1507,7 +1504,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -1518,7 +1515,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>

</xml_diff>